<commit_message>
Updated test cases and main program
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkhenderson\PycharmProjects\cs151-sky-liv_jalen_lab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bigho\PycharmProjects\cs151-sky-liv_jalen_lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9612A03-42DE-4EA2-9645-92563A16DFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12077327-43EC-42E6-94B9-879A336EE848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -531,17 +531,17 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -556,7 +556,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -598,7 +598,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -619,7 +619,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -632,7 +632,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -645,7 +645,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -666,7 +666,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -699,7 +699,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -736,7 +736,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -805,12 +805,12 @@
         <v>37.796447300922722</v>
       </c>
       <c r="J11" s="2">
-        <f>60+(H11-F11)*2</f>
-        <v>-104.40710539815456</v>
+        <f>60+(H11-F11)*1.8</f>
+        <v>-87.9663948583391</v>
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -842,8 +842,8 @@
         <v>113.38934190276817</v>
       </c>
       <c r="J12" s="2">
-        <f>60+(H12-120)*2</f>
-        <v>46.778683805536332</v>
+        <f>60+(I12-120)*1.8</f>
+        <v>48.100815424982699</v>
       </c>
       <c r="K12" s="1"/>
     </row>

</xml_diff>